<commit_message>
more bugfixes and stuff
</commit_message>
<xml_diff>
--- a/Figures/results/full_sys_1.xlsx
+++ b/Figures/results/full_sys_1.xlsx
@@ -111,6 +111,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Random DRV</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -196,13 +221,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.1951</c:v>
+                  <c:v>0.19735</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1406</c:v>
+                  <c:v>0.13625999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1145</c:v>
+                  <c:v>9.4439999999999996E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,13 +281,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.3342</c:v>
+                  <c:v>0.28194000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24640000000000001</c:v>
+                  <c:v>0.25109999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1661</c:v>
+                  <c:v>0.17230999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -277,11 +302,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="423659496"/>
-        <c:axId val="468474160"/>
+        <c:axId val="473043552"/>
+        <c:axId val="473042768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="423659496"/>
+        <c:axId val="473043552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,7 +349,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="468474160"/>
+        <c:crossAx val="473042768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -332,7 +357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="468474160"/>
+        <c:axId val="473042768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -383,7 +408,400 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423659496"/>
+        <c:crossAx val="473043552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Extreme DRVs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>spatial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$8:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>base</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mine</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>theor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$9:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>27.403600000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1123</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4619999999999997E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$8:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>base</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mine</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>theor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$10:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>37.395099999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65390000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1849999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="420918496"/>
+        <c:axId val="420924768"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="420918496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420924768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="420924768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420918496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -504,7 +922,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1012,15 +1973,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1034,6 +1995,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1308,10 +2301,13 @@
   <dimension ref="C2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
@@ -1329,13 +2325,13 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>0.1951</v>
+        <v>0.19735</v>
       </c>
       <c r="E3">
-        <v>0.1406</v>
+        <v>0.13625999999999999</v>
       </c>
       <c r="F3">
-        <v>0.1145</v>
+        <v>9.4439999999999996E-2</v>
       </c>
       <c r="H3">
         <v>0.1</v>
@@ -1352,13 +2348,13 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>0.3342</v>
+        <v>0.28194000000000002</v>
       </c>
       <c r="E4">
-        <v>0.24640000000000001</v>
+        <v>0.25109999999999999</v>
       </c>
       <c r="F4">
-        <v>0.1661</v>
+        <v>0.17230999999999999</v>
       </c>
       <c r="H4">
         <v>0.1</v>
@@ -1391,13 +2387,13 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>37.512099999999997</v>
+        <v>27.403600000000001</v>
       </c>
       <c r="E9">
-        <v>1.446</v>
+        <v>0.1123</v>
       </c>
       <c r="F9">
-        <v>1.3028999999999999</v>
+        <v>3.4619999999999997E-5</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
@@ -1405,13 +2401,13 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>53.919400000000003</v>
+        <v>37.395099999999999</v>
       </c>
       <c r="E10">
-        <v>2.4203000000000001</v>
+        <v>0.65390000000000004</v>
       </c>
       <c r="F10">
-        <v>0.69850000000000001</v>
+        <v>2.1849999999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>